<commit_message>
Adding Custom Interactable table
</commit_message>
<xml_diff>
--- a/Excels/data.xlsx
+++ b/Excels/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>RL_03_SH_0080</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Add Magical Effect to the spark</t>
   </si>
   <si>
-    <t>Vishal Mahale</t>
-  </si>
-  <si>
     <t>Brightness of spark should be reduce to 50%</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Rohit Chavan</t>
   </si>
   <si>
-    <t>Roto the fg character</t>
-  </si>
-  <si>
     <t>RL_03_SH_0869B</t>
   </si>
   <si>
@@ -190,6 +184,9 @@
   </si>
   <si>
     <t>..\thumbails\base64.txt</t>
+  </si>
+  <si>
+    <t>Roto all characters</t>
   </si>
 </sst>
 </file>
@@ -589,7 +586,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -608,34 +605,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="39.950000000000003" customHeight="1">
@@ -652,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
@@ -684,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>19</v>
@@ -714,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
@@ -744,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>19</v>
@@ -776,22 +773,22 @@
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="39.950000000000003" customHeight="1">
@@ -799,19 +796,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>11</v>
@@ -820,7 +817,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -829,23 +826,23 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H8" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1">
@@ -861,25 +858,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9" s="2">
         <v>45690.270833333336</v>

</xml_diff>